<commit_message>
commit as of 28042021
</commit_message>
<xml_diff>
--- a/data/s1.xlsx
+++ b/data/s1.xlsx
@@ -826,7 +826,7 @@
   <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -974,7 +974,7 @@
         <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>121</v>
@@ -983,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1"/>
       <c r="N2" s="4"/>
@@ -999,7 +999,7 @@
         <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>123</v>
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>137</v>
@@ -1086,7 +1086,7 @@
         <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>130</v>
@@ -1138,7 +1138,7 @@
         <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>
@@ -1177,7 +1177,7 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>138</v>
@@ -1248,7 +1248,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>142</v>

</xml_diff>